<commit_message>
Committing the 7 test cases scripts for the CCDI studies phs000466 and phs000467
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs002790.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs002790.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjanya0307\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\03-31-25\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46989D3-9639-4BE7-80B3-C772FCBD17E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00ECA7A-FC57-4911-AA36-4E6C9804ABBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>WebExcel</t>
   </si>
@@ -116,26 +116,6 @@
 left join files f on s.study_id = f.study_id
 left join personnel pr on s.study_id = pr.study_id
 left join funding f on s.study_id = f.study </t>
-  </si>
-  <si>
-    <t>SELECT
-    COUNT(DISTINCT s.dbgap_accession) AS "Studies",
-    COUNT(DISTINCT p.participant_id) AS "Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Samples",
-    (COUNT(DISTINCT seq.id) + COUNT(DISTINCT maf.id) + COUNT(DISTINCT cmf.id) + COUNT(DISTINCT path.id)) AS "Files"
-FROM 
-    from study s
-left join diagnosis d on s.study_id = d.study_id
-left join participants p on s.study_id = p.study_id
-left join sample smp on s.study_id = smp.study_id
-left join sequencing_file seq on s.study_id = seq.study_id
-left join methylation_array_file maf on s.study_id = maf.study_id
-left join pathology_file path on s.study_id = path.study_id
-left join clinical_measure_file cmf on s.study_id = cmf.study_id
-left join personnel pr on s.study_id = pr.study_id
-left join funding f on s.study_id = f.study 
-WHERE 
-    std.dbgap_accession = 'phs002790';</t>
   </si>
   <si>
     <t>with diagnosis1 as (
@@ -267,21 +247,1157 @@
     std.dbgap_accession = 'phs002790'
 ;</t>
   </si>
+  <si>
+    <r>
+      <t>    COUNT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DISTINCT std</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dbgap_accession</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> AS "Studies"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    COUNT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DISTINCT prt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>participant_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> AS "Participants"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    COUNT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DISTINCT smp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sample_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> AS "Samples"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    COALESCE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        COUNT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DISTINCT sequ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        COUNT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DISTINCT methyl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        COUNT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DISTINCT patho</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        COUNT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DISTINCT cmf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>),</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> AS "Files"</t>
+    </r>
+  </si>
+  <si>
+    <t>FROM </t>
+  </si>
+  <si>
+    <t>    df_study std</t>
+  </si>
+  <si>
+    <t>LEFT JOIN </t>
+  </si>
+  <si>
+    <r>
+      <t>    df_participant prt ON std</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> prt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"study.id"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    df_sample smp ON prt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> smp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"participant.id"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    df_diagnosis diag ON prt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> diag</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"participant.id"     </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    df_clinical_measure_file cmf ON prt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> cmf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"participant.id"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    df_sequencing_file sequ ON smp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> sequ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"sample.id"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    df_methylation_array_file methyl ON smp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> methyl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"sample.id"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    df_pathology_file patho ON smp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> patho</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"sample.id"</t>
+    </r>
+  </si>
+  <si>
+    <t>WHERE </t>
+  </si>
+  <si>
+    <r>
+      <t>    std</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dbgap_accession </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 'phs002790'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF37797B"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>SELECT
+    COUNT(DISTINCT std.dbgap_accession) AS "Studies",
+    COUNT(DISTINCT prt.participant_id) AS "Participants",
+    COUNT(DISTINCT smp.sample_id) AS "Samples",
+    COALESCE(
+        COUNT(DISTINCT sequ.file_name) + 
+        COUNT(DISTINCT methyl.file_name) + 
+        COUNT(DISTINCT patho.file_name) + 
+        COUNT(DISTINCT cmf.file_name),
+        0
+    ) AS "Files"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_sample smp ON prt.id = smp."participant.id"
+LEFT JOIN 
+    df_diagnosis diag ON prt.id = diag."participant.id"     
+LEFT JOIN 
+    df_clinical_measure_file cmf ON prt.id = cmf."participant.id"
+LEFT JOIN 
+    df_sequencing_file sequ ON smp.id = sequ."sample.id"
+LEFT JOIN 
+    df_methylation_array_file methyl ON smp.id = methyl."sample.id"
+LEFT JOIN 
+    df_pathology_file patho ON smp.id = patho."sample.id"
+WHERE 
+    std.dbgap_accession = 'phs002790';</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -308,8 +1424,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF37797B"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -334,17 +1450,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -665,10 +1775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,11 +1810,11 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -717,38 +1827,167 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
ICDC - OSA04 and CCDI - phs000463
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs002790.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs002790.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\sowjanya0307\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46989D3-9639-4BE7-80B3-C772FCBD17E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7041432-D615-4205-A822-E3F7016C8AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,26 +118,6 @@
 left join funding f on s.study_id = f.study </t>
   </si>
   <si>
-    <t>SELECT
-    COUNT(DISTINCT s.dbgap_accession) AS "Studies",
-    COUNT(DISTINCT p.participant_id) AS "Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Samples",
-    (COUNT(DISTINCT seq.id) + COUNT(DISTINCT maf.id) + COUNT(DISTINCT cmf.id) + COUNT(DISTINCT path.id)) AS "Files"
-FROM 
-    from study s
-left join diagnosis d on s.study_id = d.study_id
-left join participants p on s.study_id = p.study_id
-left join sample smp on s.study_id = smp.study_id
-left join sequencing_file seq on s.study_id = seq.study_id
-left join methylation_array_file maf on s.study_id = maf.study_id
-left join pathology_file path on s.study_id = path.study_id
-left join clinical_measure_file cmf on s.study_id = cmf.study_id
-left join personnel pr on s.study_id = pr.study_id
-left join funding f on s.study_id = f.study 
-WHERE 
-    std.dbgap_accession = 'phs002790';</t>
-  </si>
-  <si>
     <t>with diagnosis1 as (
 select dgn."participant.id", group_concat(dgn.age_at_diagnosis,';') as age, group_concat(dgn.diagnosis,';') as diag,group_concat(dgn.anatomic_site,';') as ant_site from df_diagnosis dgn where dgn."participant.id" is not null group by dgn."participant.id" ),
 diagnosis2 as (select "participant.id",  group_concat(diagnosis,';') as diag from (select distinct "participant.id", diagnosis from df_diagnosis  where "participant.id" is not null )  group by "participant.id" ),
@@ -266,6 +246,37 @@
 WHERE 
     std.dbgap_accession = 'phs002790'
 ;</t>
+  </si>
+  <si>
+    <t>SELECT
+    COUNT(DISTINCT std.dbgap_accession) AS "Studies",
+    COUNT(DISTINCT prt.participant_id) AS "Participants",
+    COUNT(DISTINCT smp.sample_id) AS "Samples",
+    COALESCE(
+        COUNT(DISTINCT sequ.id) + 
+        COUNT(DISTINCT methyl.id) + 
+        COUNT(DISTINCT patho.id) + 
+        COUNT(DISTINCT cmf.id),
+        0
+    ) AS "Files"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_sample smp ON prt.id = smp."participant.id"
+LEFT JOIN 
+    df_diagnosis diag ON prt.id = diag."participant.id"     
+LEFT JOIN 
+    df_clinical_measure_file cmf ON prt.id = cmf."participant.id"
+LEFT JOIN 
+    df_sequencing_file sequ ON smp.id = sequ."sample.id"
+LEFT JOIN 
+    df_methylation_array_file methyl ON smp.id = methyl."sample.id"
+LEFT JOIN 
+    df_pathology_file patho ON smp.id = patho."sample.id"
+WHERE 
+    std.dbgap_accession = 'phs002790';</t>
   </si>
 </sst>
 </file>
@@ -667,19 +678,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.85546875" customWidth="1"/>
-    <col min="4" max="4" width="70.140625" customWidth="1"/>
-    <col min="5" max="5" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.88671875" customWidth="1"/>
+    <col min="4" max="4" width="70.109375" customWidth="1"/>
+    <col min="5" max="5" width="63.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -696,15 +707,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -713,7 +724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -722,29 +733,29 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
     </row>
   </sheetData>

</xml_diff>